<commit_message>
add sentiment and comment length features.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/stats/datasets.xlsx
+++ b/src/main/resources/data/stats/datasets.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1DC335-093F-456F-8889-0AD67EF08BC7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF39D3A3-0523-4BE9-8805-DACDB5F3AA28}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>language</t>
   </si>
@@ -260,12 +260,21 @@
   </si>
   <si>
     <t>Top 10 Tokens (broken)</t>
+  </si>
+  <si>
+    <t>token per comment ratio</t>
+  </si>
+  <si>
+    <t>positive comment ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -387,25 +396,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -689,20 +702,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:NR65"/>
+  <dimension ref="A1:NR67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="18.26953125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>53</v>
       </c>
@@ -713,14 +726,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>73</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -733,7 +746,7 @@
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:382" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:382" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -746,19 +759,19 @@
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
@@ -804,7 +817,7 @@
       <c r="NF8" s="1"/>
       <c r="NJ8" s="1"/>
     </row>
-    <row r="9" spans="1:382" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:382" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>56</v>
       </c>
@@ -879,559 +892,582 @@
       <c r="NN9" s="1"/>
       <c r="NR9" s="1"/>
     </row>
-    <row r="10" spans="1:382" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:382" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="18">
         <v>0.33269496799999998</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0.99433333300000004</v>
       </c>
     </row>
-    <row r="11" spans="1:382" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:382" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+    <row r="11" spans="1:382" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="20">
+        <v>0.329928715820832</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:382" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:382" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:382" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:382" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B14" s="9">
         <v>28575</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C14" s="9">
         <v>41025</v>
       </c>
     </row>
-    <row r="14" spans="1:382" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:382" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15" s="5">
         <v>3921</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C15" s="5">
         <v>6127</v>
       </c>
     </row>
-    <row r="15" spans="1:382" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+    <row r="16" spans="1:382" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B16" s="18">
         <v>0.137217848</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C16" s="18">
         <v>0.149347959</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="G16" s="24"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="26">
+        <v>3.0402170439999998</v>
+      </c>
+      <c r="C17" s="26">
+        <v>13.675000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B20" s="9">
         <v>12</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C20" s="9">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B24" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B25" s="18">
         <v>0.34624671899999998</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C25" s="18">
         <v>0.17199268700000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C26" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B27" s="19">
         <v>0.19251093599999999</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C27" s="19">
         <v>0.159707495</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B29" s="19">
         <v>8.2239720000000002E-2</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C29" s="19">
         <v>0.13272394900000001</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B31" s="19">
         <v>6.6246718999999996E-2</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C31" s="19">
         <v>0.106837294</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="24">
+      <c r="B33" s="20">
         <v>6.5896762999999997E-2</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C33" s="20">
         <v>0.10166971399999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="22">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="21"/>
+      <c r="B37" s="18">
         <v>0.51846169581671198</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C37" s="18">
         <v>6.8208422555317602E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B38" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="23">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="21"/>
+      <c r="B39" s="19">
         <v>0.118952643960315</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C39" s="19">
         <v>6.0870806566738003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="23">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="21"/>
+      <c r="B41" s="19">
         <v>9.6144011455456604E-2</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C41" s="19">
         <v>4.9193433261955702E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="23">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="21"/>
+      <c r="B43" s="19">
         <v>9.0007159660427494E-2</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C43" s="19">
         <v>4.7052105638829403E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="24">
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="22"/>
+      <c r="B45" s="20">
         <v>7.6608366574613895E-2</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C45" s="20">
         <v>4.2084225553176299E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B48" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B49" s="5">
         <v>0.16888888899999999</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C49" s="5">
         <v>7.4149909E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C50" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B51" s="5">
         <v>0.168853893</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C51" s="5">
         <v>3.6026812999999998E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="C52" s="5"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B53" s="5">
         <v>1.6447943999999999E-2</v>
       </c>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B54" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C54" s="5">
         <v>3.1834247000000003E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B55" s="5">
         <v>1.4628171000000001E-2</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5">
         <v>2.7007922E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B58" s="5">
         <v>1.3088364E-2</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C58" s="5">
         <v>2.0938452E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B60" s="5">
         <v>1.2283465E-2</v>
       </c>
-      <c r="C58" s="5">
+      <c r="C60" s="5">
         <v>2.0694698000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B61" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B62" s="5">
         <v>1.1513561E-2</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C62" s="5">
         <v>1.8281536000000001E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B63" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B64" s="5">
         <v>9.5188100000000008E-3</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C64" s="5">
         <v>1.6087751000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B65" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
+    <row r="67" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="12">
+      <c r="B67" s="12">
         <v>6.9991250000000001E-3</v>
       </c>
-      <c r="C65" s="12">
+      <c r="C67" s="12">
         <v>1.3820841E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
     <mergeCell ref="A60:A61"/>
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A66:A67"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A58:A59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>